<commit_message>
prise en compte décision aout et relecture Guillaume (#110)
* prise en compte décision aout et relecture Guillaume

* correction exemple pour inclure authoredOn

* MàJ liste particpants

* Fix exemple Nicoretteskin

* last work

* correction sur last batch

* Correction liens cd4a9267e4d96fce929ac3f7dbed770b6fec394d
</commit_message>
<xml_diff>
--- a/main/ig/PN13-FHIR-FreeSetCIODC-Unite-ConceptMap.xlsx
+++ b/main/ig/PN13-FHIR-FreeSetCIODC-Unite-ConceptMap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="286">
   <si>
     <t>Property</t>
   </si>
@@ -127,33 +127,12 @@
     <t>10n</t>
   </si>
   <si>
-    <t>10*6.a</t>
-  </si>
-  <si>
-    <t>M[arb'U]</t>
-  </si>
-  <si>
-    <t>106U</t>
-  </si>
-  <si>
     <t>10*6.bq</t>
   </si>
   <si>
     <t>MBq</t>
   </si>
   <si>
-    <t>10*6.iu</t>
-  </si>
-  <si>
-    <t>M[iU]</t>
-  </si>
-  <si>
-    <t>106UI</t>
-  </si>
-  <si>
-    <t>10*6.u</t>
-  </si>
-  <si>
     <t>10*9</t>
   </si>
   <si>
@@ -166,591 +145,228 @@
     <t>GBq</t>
   </si>
   <si>
-    <t>agD_u</t>
-  </si>
-  <si>
-    <t>[D'ag'U]</t>
-  </si>
-  <si>
-    <t>U agD</t>
-  </si>
-  <si>
-    <t>ah_u</t>
-  </si>
-  <si>
-    <t>[arb'U]{anti'hep}</t>
-  </si>
-  <si>
-    <t>U anti hép.</t>
-  </si>
-  <si>
     <t>an</t>
   </si>
   <si>
     <t>a</t>
   </si>
   <si>
-    <t>arb_u</t>
-  </si>
-  <si>
-    <t>[arb'U]</t>
+    <t>bq</t>
+  </si>
+  <si>
+    <t>Bq</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>g/h</t>
+  </si>
+  <si>
+    <t>g/kg</t>
+  </si>
+  <si>
+    <t>g/kg/h</t>
+  </si>
+  <si>
+    <t>g/kg/mn</t>
+  </si>
+  <si>
+    <t>g/kg/min</t>
+  </si>
+  <si>
+    <t>g/m2</t>
+  </si>
+  <si>
+    <t>g/m²</t>
+  </si>
+  <si>
+    <t>g/m2/h</t>
+  </si>
+  <si>
+    <t>g/m²/h</t>
+  </si>
+  <si>
+    <t>g/m2/mn</t>
+  </si>
+  <si>
+    <t>g/m2/min</t>
+  </si>
+  <si>
+    <t>g/m²/min</t>
+  </si>
+  <si>
+    <t>g/mn</t>
+  </si>
+  <si>
+    <t>g/min</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L/mn</t>
+  </si>
+  <si>
+    <t>L/min</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m²</t>
+  </si>
+  <si>
+    <t>meq</t>
+  </si>
+  <si>
+    <t>meq/L</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>mg/h</t>
+  </si>
+  <si>
+    <t>mg/kg</t>
+  </si>
+  <si>
+    <t>mg/kg/h</t>
+  </si>
+  <si>
+    <t>mg/kg/mn</t>
+  </si>
+  <si>
+    <t>mg/kg/min</t>
+  </si>
+  <si>
+    <t>mg/m2</t>
+  </si>
+  <si>
+    <t>mg/m²</t>
+  </si>
+  <si>
+    <t>mg/m2/h</t>
+  </si>
+  <si>
+    <t>mg/m²/h</t>
+  </si>
+  <si>
+    <t>mg/m2/mn</t>
+  </si>
+  <si>
+    <t>mg/m2/min</t>
+  </si>
+  <si>
+    <t>mg/m²/min</t>
+  </si>
+  <si>
+    <t>mg/mn</t>
+  </si>
+  <si>
+    <t>mg/min</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>mL/h</t>
+  </si>
+  <si>
+    <t>mL/kg</t>
+  </si>
+  <si>
+    <t>mL/kg/h</t>
+  </si>
+  <si>
+    <t>mL/kg/mn</t>
+  </si>
+  <si>
+    <t>mL/kg/min</t>
+  </si>
+  <si>
+    <t>mL/m2</t>
+  </si>
+  <si>
+    <t>mL/m²</t>
+  </si>
+  <si>
+    <t>mL/m2/h</t>
+  </si>
+  <si>
+    <t>mL/m²/h</t>
+  </si>
+  <si>
+    <t>mL/m2/mn</t>
+  </si>
+  <si>
+    <t>mL/m2/min</t>
+  </si>
+  <si>
+    <t>mL/m²/min</t>
+  </si>
+  <si>
+    <t>mL/mn</t>
+  </si>
+  <si>
+    <t>mL/min</t>
+  </si>
+  <si>
+    <t>mmol</t>
+  </si>
+  <si>
+    <t>mmol/L</t>
+  </si>
+  <si>
+    <t>mn</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>mois</t>
+  </si>
+  <si>
+    <t>mo</t>
+  </si>
+  <si>
+    <t>mosm/L</t>
+  </si>
+  <si>
+    <t>ng</t>
+  </si>
+  <si>
+    <t>ng/kg/mn</t>
+  </si>
+  <si>
+    <t>ng/kg/min</t>
+  </si>
+  <si>
+    <t>nkat</t>
+  </si>
+  <si>
+    <t>u</t>
   </si>
   <si>
     <t>U</t>
   </si>
   <si>
-    <t>axa_iu</t>
-  </si>
-  <si>
-    <t>[anti'Xa'U]</t>
-  </si>
-  <si>
-    <t>U anti Xa</t>
-  </si>
-  <si>
-    <t>boite</t>
-  </si>
-  <si>
-    <t>{box}</t>
-  </si>
-  <si>
-    <t>boîte</t>
-  </si>
-  <si>
-    <t>bq</t>
-  </si>
-  <si>
-    <t>Bq</t>
-  </si>
-  <si>
-    <t>c_a_c</t>
-  </si>
-  <si>
-    <t>[tsp_m]</t>
-  </si>
-  <si>
-    <t>càc</t>
-  </si>
-  <si>
-    <t>c_a_d</t>
-  </si>
-  <si>
-    <t>{dsp}</t>
-  </si>
-  <si>
-    <t>càd</t>
-  </si>
-  <si>
-    <t>c_a_s</t>
-  </si>
-  <si>
-    <t>[tbs_m]</t>
-  </si>
-  <si>
-    <t>càs</t>
-  </si>
-  <si>
-    <t>cadre</t>
-  </si>
-  <si>
-    <t>{frame}</t>
-  </si>
-  <si>
-    <t>caisse</t>
-  </si>
-  <si>
-    <t>{crate}</t>
-  </si>
-  <si>
-    <t>ceip_u</t>
-  </si>
-  <si>
-    <t>[arb'U]{ceip}</t>
-  </si>
-  <si>
-    <t>U CEIP</t>
-  </si>
-  <si>
-    <t>cycle</t>
-  </si>
-  <si>
-    <t>{cycle}</t>
-  </si>
-  <si>
-    <t>ddose</t>
-  </si>
-  <si>
-    <t>{meas'dev}</t>
-  </si>
-  <si>
-    <t>disp.doseur</t>
-  </si>
-  <si>
-    <t>dose</t>
-  </si>
-  <si>
-    <t>{dose}</t>
-  </si>
-  <si>
-    <t>dose_kg</t>
-  </si>
-  <si>
-    <t>{kg'dose}</t>
-  </si>
-  <si>
-    <t>dose-kg</t>
-  </si>
-  <si>
-    <t>dosevac</t>
-  </si>
-  <si>
-    <t>{vac'dose}</t>
-  </si>
-  <si>
-    <t>dose-vac</t>
-  </si>
-  <si>
-    <t>eph_u</t>
-  </si>
-  <si>
-    <t>[arb'U]{eph}</t>
-  </si>
-  <si>
-    <t>UPE</t>
-  </si>
-  <si>
-    <t>feiba_u</t>
-  </si>
-  <si>
-    <t>[arb'U]{feiba}</t>
-  </si>
-  <si>
-    <t>U FEIBA</t>
-  </si>
-  <si>
-    <t>feuille</t>
-  </si>
-  <si>
-    <t>{foil}</t>
-  </si>
-  <si>
-    <t>flac c-gttes</t>
-  </si>
-  <si>
-    <t>{drpr'cont}</t>
-  </si>
-  <si>
-    <t>flac.c.gttes</t>
-  </si>
-  <si>
-    <t>flac_pres</t>
-  </si>
-  <si>
-    <t>{prsrd'cont}</t>
-  </si>
-  <si>
-    <t>flac.press.</t>
-  </si>
-  <si>
-    <t>flac_pulv</t>
-  </si>
-  <si>
-    <t>{spray}</t>
-  </si>
-  <si>
-    <t>flac.pulv.</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>g/h</t>
-  </si>
-  <si>
-    <t>g/kg</t>
-  </si>
-  <si>
-    <t>g/kg/h</t>
-  </si>
-  <si>
-    <t>g/kg/mn</t>
-  </si>
-  <si>
-    <t>g/kg/min</t>
-  </si>
-  <si>
-    <t>g/m2</t>
-  </si>
-  <si>
-    <t>g/m²</t>
-  </si>
-  <si>
-    <t>g/m2/h</t>
-  </si>
-  <si>
-    <t>g/m²/h</t>
-  </si>
-  <si>
-    <t>g/m2/mn</t>
-  </si>
-  <si>
-    <t>g/m2/min</t>
-  </si>
-  <si>
-    <t>g/m²/min</t>
-  </si>
-  <si>
-    <t>g/mn</t>
-  </si>
-  <si>
-    <t>g/min</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>inka_u</t>
-  </si>
-  <si>
-    <t>[arb'U]{kallikrein inactivator}</t>
-  </si>
-  <si>
-    <t>U IK</t>
-  </si>
-  <si>
-    <t>iu</t>
-  </si>
-  <si>
-    <t>[iU]</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>iu/h</t>
-  </si>
-  <si>
-    <t>[iU]/h</t>
-  </si>
-  <si>
-    <t>UI/h</t>
-  </si>
-  <si>
-    <t>iu/kg</t>
-  </si>
-  <si>
-    <t>[iU]/kg</t>
-  </si>
-  <si>
-    <t>UI/kg</t>
-  </si>
-  <si>
-    <t>iu/kg/h</t>
-  </si>
-  <si>
-    <t>[iU]/kg/h</t>
-  </si>
-  <si>
-    <t>UI/kg/h</t>
-  </si>
-  <si>
-    <t>iu/kg/mn</t>
-  </si>
-  <si>
-    <t>[iU]/kg/min</t>
-  </si>
-  <si>
-    <t>UI/kg/min</t>
-  </si>
-  <si>
-    <t>iu/m2</t>
-  </si>
-  <si>
-    <t>[iU]/m2</t>
-  </si>
-  <si>
-    <t>UI/m²</t>
-  </si>
-  <si>
-    <t>iu/m2/h</t>
-  </si>
-  <si>
-    <t>[iU]/m2/h</t>
-  </si>
-  <si>
-    <t>UI/m²/h</t>
-  </si>
-  <si>
-    <t>iu/m2/mn</t>
-  </si>
-  <si>
-    <t>[iU]/m2/min</t>
-  </si>
-  <si>
-    <t>UI/m²/min</t>
-  </si>
-  <si>
-    <t>iu/mL</t>
-  </si>
-  <si>
-    <t>[iU]/mL</t>
-  </si>
-  <si>
-    <t>UI/mL</t>
-  </si>
-  <si>
-    <t>iu/mn</t>
-  </si>
-  <si>
-    <t>[iU]/min</t>
-  </si>
-  <si>
-    <t>UI/min</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>kit</t>
-  </si>
-  <si>
-    <t>{kit}</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L/mn</t>
-  </si>
-  <si>
-    <t>L/min</t>
-  </si>
-  <si>
-    <t>loo_u</t>
-  </si>
-  <si>
-    <t>[arb'U]{loo}</t>
-  </si>
-  <si>
-    <t>Loomis</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
-    <t>m²</t>
-  </si>
-  <si>
-    <t>meq</t>
-  </si>
-  <si>
-    <t>meq/L</t>
-  </si>
-  <si>
-    <t>mg</t>
-  </si>
-  <si>
-    <t>mg/h</t>
-  </si>
-  <si>
-    <t>mg/kg</t>
-  </si>
-  <si>
-    <t>mg/kg/h</t>
-  </si>
-  <si>
-    <t>mg/kg/mn</t>
-  </si>
-  <si>
-    <t>mg/kg/min</t>
-  </si>
-  <si>
-    <t>mg/m2</t>
-  </si>
-  <si>
-    <t>mg/m²</t>
-  </si>
-  <si>
-    <t>mg/m2/h</t>
-  </si>
-  <si>
-    <t>mg/m²/h</t>
-  </si>
-  <si>
-    <t>mg/m2/mn</t>
-  </si>
-  <si>
-    <t>mg/m2/min</t>
-  </si>
-  <si>
-    <t>mg/m²/min</t>
-  </si>
-  <si>
-    <t>mg/mn</t>
-  </si>
-  <si>
-    <t>mg/min</t>
-  </si>
-  <si>
-    <t>mL</t>
-  </si>
-  <si>
-    <t>mL/h</t>
-  </si>
-  <si>
-    <t>mL/kg</t>
-  </si>
-  <si>
-    <t>mL/kg/h</t>
-  </si>
-  <si>
-    <t>mL/kg/mn</t>
-  </si>
-  <si>
-    <t>mL/kg/min</t>
-  </si>
-  <si>
-    <t>mL/m2</t>
-  </si>
-  <si>
-    <t>mL/m²</t>
-  </si>
-  <si>
-    <t>mL/m2/h</t>
-  </si>
-  <si>
-    <t>mL/m²/h</t>
-  </si>
-  <si>
-    <t>mL/m2/mn</t>
-  </si>
-  <si>
-    <t>mL/m2/min</t>
-  </si>
-  <si>
-    <t>mL/m²/min</t>
-  </si>
-  <si>
-    <t>mL/mn</t>
-  </si>
-  <si>
-    <t>mL/min</t>
-  </si>
-  <si>
-    <t>mmol</t>
-  </si>
-  <si>
-    <t>mmol/L</t>
-  </si>
-  <si>
-    <t>mn</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>mois</t>
-  </si>
-  <si>
-    <t>mo</t>
-  </si>
-  <si>
-    <t>mosm/L</t>
-  </si>
-  <si>
-    <t>ng</t>
-  </si>
-  <si>
-    <t>ng/kg/mn</t>
-  </si>
-  <si>
-    <t>ng/kg/min</t>
-  </si>
-  <si>
-    <t>nkat</t>
-  </si>
-  <si>
-    <t>paire</t>
-  </si>
-  <si>
-    <t>{pair}</t>
-  </si>
-  <si>
-    <t>pièce</t>
-  </si>
-  <si>
-    <t>{piece}</t>
-  </si>
-  <si>
-    <t>ppe_doseuse</t>
-  </si>
-  <si>
-    <t>{meter'pump}</t>
-  </si>
-  <si>
-    <t>pompe doseuse</t>
-  </si>
-  <si>
-    <t>pres</t>
-  </si>
-  <si>
-    <t>{press}</t>
-  </si>
-  <si>
-    <t>pression</t>
-  </si>
-  <si>
-    <t>pst</t>
-  </si>
-  <si>
-    <t>{bandg}</t>
-  </si>
-  <si>
-    <t>rec_dose</t>
-  </si>
-  <si>
-    <t>{meter'cont}</t>
-  </si>
-  <si>
-    <t>récip.doseur</t>
-  </si>
-  <si>
-    <t>rec_multi</t>
-  </si>
-  <si>
-    <t>{multidose'cont}</t>
-  </si>
-  <si>
-    <t>récip.multidose</t>
-  </si>
-  <si>
-    <t>rec_unidose</t>
-  </si>
-  <si>
-    <t>{sgldose'cont}</t>
-  </si>
-  <si>
-    <t>récip.unidose</t>
-  </si>
-  <si>
-    <t>set</t>
-  </si>
-  <si>
-    <t>{set}</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
     <t>ug</t>
   </si>
   <si>
@@ -833,15 +449,6 @@
   </si>
   <si>
     <t>µL</t>
-  </si>
-  <si>
-    <t>VAPO</t>
-  </si>
-  <si>
-    <t>{evaporator}</t>
-  </si>
-  <si>
-    <t>évaporateur</t>
   </si>
   <si>
     <t>http://standardterms.edqm.eu</t>
@@ -1521,7 +1128,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1603,57 +1210,57 @@
         <v>38</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -1663,1582 +1270,862 @@
         <v>46</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s" s="2">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s" s="2">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s" s="2">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="E28" t="s" s="2">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="E29" t="s" s="2">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s" s="2">
-        <v>103</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E31" t="s" s="2">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="E32" t="s" s="2">
-        <v>108</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s" s="2">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="E34" t="s" s="2">
-        <v>114</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="E35" t="s" s="2">
-        <v>115</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D36" t="s" s="2">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s" s="2">
-        <v>116</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s" s="2">
-        <v>117</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D38" t="s" s="2">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="E38" t="s" s="2">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="E39" t="s" s="2">
-        <v>120</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D40" t="s" s="2">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="E40" t="s" s="2">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="E41" t="s" s="2">
-        <v>124</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="E42" t="s" s="2">
-        <v>127</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E43" t="s" s="2">
-        <v>129</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D44" t="s" s="2">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E44" t="s" s="2">
-        <v>130</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="E45" t="s" s="2">
-        <v>133</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D46" t="s" s="2">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="E46" t="s" s="2">
-        <v>136</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D47" t="s" s="2">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="E47" t="s" s="2">
-        <v>139</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="E48" t="s" s="2">
-        <v>142</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="E49" t="s" s="2">
-        <v>145</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="E50" t="s" s="2">
-        <v>148</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D51" t="s" s="2">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="E51" t="s" s="2">
-        <v>151</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D52" t="s" s="2">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="E52" t="s" s="2">
-        <v>154</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D53" t="s" s="2">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="E53" t="s" s="2">
-        <v>157</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D54" t="s" s="2">
-        <v>159</v>
+        <v>116</v>
       </c>
       <c r="E54" t="s" s="2">
-        <v>160</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D55" t="s" s="2">
-        <v>162</v>
+        <v>117</v>
       </c>
       <c r="E55" t="s" s="2">
-        <v>163</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D56" t="s" s="2">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="E56" t="s" s="2">
-        <v>164</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D57" t="s" s="2">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="E57" t="s" s="2">
-        <v>166</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D58" t="s" s="2">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="E58" t="s" s="2">
-        <v>167</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D59" t="s" s="2">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="E59" t="s" s="2">
-        <v>169</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D60" t="s" s="2">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="E60" t="s" s="2">
-        <v>171</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D61" t="s" s="2">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="E61" t="s" s="2">
-        <v>174</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>175</v>
+        <v>132</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D62" t="s" s="2">
-        <v>175</v>
+        <v>133</v>
       </c>
       <c r="E62" t="s" s="2">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D63" t="s" s="2">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="E63" t="s" s="2">
-        <v>177</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D64" t="s" s="2">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="E64" t="s" s="2">
-        <v>178</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D65" t="s" s="2">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="E65" t="s" s="2">
-        <v>179</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D66" t="s" s="2">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="E66" t="s" s="2">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D67" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="E67" t="s" s="2">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D68" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="E68" t="s" s="2">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="B69" s="2"/>
-      <c r="C69" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D69" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="E69" t="s" s="2">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="B70" s="2"/>
-      <c r="C70" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D70" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="E70" t="s" s="2">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D71" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="E71" t="s" s="2">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D72" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="E72" t="s" s="2">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D73" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="E73" t="s" s="2">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D74" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="E74" t="s" s="2">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D75" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="E75" t="s" s="2">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D76" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="E76" t="s" s="2">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="B77" s="2"/>
-      <c r="C77" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D77" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="E77" t="s" s="2">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="B78" s="2"/>
-      <c r="C78" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D78" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="E78" t="s" s="2">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="B79" s="2"/>
-      <c r="C79" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D79" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="E79" t="s" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D80" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="E80" t="s" s="2">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="B81" s="2"/>
-      <c r="C81" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D81" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E81" t="s" s="2">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="B82" s="2"/>
-      <c r="C82" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D82" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="E82" t="s" s="2">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="B83" s="2"/>
-      <c r="C83" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D83" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="E83" t="s" s="2">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="B84" s="2"/>
-      <c r="C84" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D84" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="E84" t="s" s="2">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="B85" s="2"/>
-      <c r="C85" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D85" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="E85" t="s" s="2">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="B86" s="2"/>
-      <c r="C86" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D86" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="E86" t="s" s="2">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="B87" s="2"/>
-      <c r="C87" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D87" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="E87" t="s" s="2">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="B88" s="2"/>
-      <c r="C88" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D88" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="E88" t="s" s="2">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="B89" s="2"/>
-      <c r="C89" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D89" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="E89" t="s" s="2">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="B90" s="2"/>
-      <c r="C90" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D90" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="E90" t="s" s="2">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="B91" s="2"/>
-      <c r="C91" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D91" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="E91" t="s" s="2">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="B92" s="2"/>
-      <c r="C92" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D92" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="E92" t="s" s="2">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="B93" s="2"/>
-      <c r="C93" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D93" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="E93" t="s" s="2">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="B94" s="2"/>
-      <c r="C94" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D94" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="E94" t="s" s="2">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="B95" s="2"/>
-      <c r="C95" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D95" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="E95" t="s" s="2">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="B96" s="2"/>
-      <c r="C96" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D96" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="E96" t="s" s="2">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="B97" s="2"/>
-      <c r="C97" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D97" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="E97" t="s" s="2">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="B98" s="2"/>
-      <c r="C98" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D98" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="E98" t="s" s="2">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="B99" s="2"/>
-      <c r="C99" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D99" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="E99" t="s" s="2">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="B100" s="2"/>
-      <c r="C100" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D100" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="E100" t="s" s="2">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="B101" s="2"/>
-      <c r="C101" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D101" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="E101" t="s" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="B102" s="2"/>
-      <c r="C102" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D102" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="E102" t="s" s="2">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="B103" s="2"/>
-      <c r="C103" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D103" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="E103" t="s" s="2">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="B104" s="2"/>
-      <c r="C104" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D104" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="E104" t="s" s="2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="B105" s="2"/>
-      <c r="C105" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D105" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="E105" t="s" s="2">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="B106" s="2"/>
-      <c r="C106" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D106" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="E106" t="s" s="2">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="B107" s="2"/>
-      <c r="C107" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D107" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="E107" t="s" s="2">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="B108" s="2"/>
-      <c r="C108" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D108" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="E108" t="s" s="2">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="B109" s="2"/>
-      <c r="C109" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D109" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="E109" t="s" s="2">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="B110" s="2"/>
-      <c r="C110" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D110" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="E110" t="s" s="2">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="B111" s="2"/>
-      <c r="C111" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D111" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="E111" t="s" s="2">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="B112" s="2"/>
-      <c r="C112" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D112" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="E112" t="s" s="2">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="B113" s="2"/>
-      <c r="C113" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D113" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="E113" t="s" s="2">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="B114" s="2"/>
-      <c r="C114" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="D114" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="E114" t="s" s="2">
-        <v>275</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3282,7 +2169,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>276</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>30</v>
@@ -3290,782 +2177,782 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>277</v>
+        <v>146</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>278</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>279</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>280</v>
+        <v>149</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>281</v>
+        <v>150</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>282</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>283</v>
+        <v>152</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>284</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>285</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>286</v>
+        <v>155</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>287</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>288</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>289</v>
+        <v>158</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>290</v>
+        <v>159</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>291</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>292</v>
+        <v>161</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>293</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>294</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>295</v>
+        <v>164</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>296</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>297</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>298</v>
+        <v>167</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>299</v>
+        <v>168</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>300</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>301</v>
+        <v>170</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>302</v>
+        <v>171</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>303</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>304</v>
+        <v>173</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>305</v>
+        <v>174</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>306</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>307</v>
+        <v>176</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>308</v>
+        <v>177</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>309</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>310</v>
+        <v>179</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>311</v>
+        <v>180</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>312</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>313</v>
+        <v>182</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>314</v>
+        <v>183</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>315</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>316</v>
+        <v>185</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>317</v>
+        <v>186</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>318</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>319</v>
+        <v>188</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>320</v>
+        <v>189</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>321</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>322</v>
+        <v>191</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>317</v>
+        <v>186</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>318</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>323</v>
+        <v>192</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>320</v>
+        <v>189</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>321</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>324</v>
+        <v>193</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>325</v>
+        <v>194</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>326</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>327</v>
+        <v>196</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>328</v>
+        <v>197</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>329</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>330</v>
+        <v>199</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>331</v>
+        <v>200</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>332</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>333</v>
+        <v>202</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>334</v>
+        <v>203</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>297</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>335</v>
+        <v>204</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>336</v>
+        <v>205</v>
       </c>
       <c r="E24" t="s" s="2">
-        <v>337</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>338</v>
+        <v>207</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>339</v>
+        <v>208</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>340</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>341</v>
+        <v>210</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>302</v>
+        <v>171</v>
       </c>
       <c r="E26" t="s" s="2">
-        <v>342</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>343</v>
+        <v>212</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>344</v>
+        <v>213</v>
       </c>
       <c r="E27" t="s" s="2">
-        <v>345</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>346</v>
+        <v>215</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>347</v>
+        <v>216</v>
       </c>
       <c r="E28" t="s" s="2">
-        <v>348</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>349</v>
+        <v>218</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>350</v>
+        <v>219</v>
       </c>
       <c r="E29" t="s" s="2">
-        <v>351</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>352</v>
+        <v>221</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>353</v>
+        <v>222</v>
       </c>
       <c r="E30" t="s" s="2">
-        <v>354</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>355</v>
+        <v>224</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>356</v>
+        <v>225</v>
       </c>
       <c r="E31" t="s" s="2">
-        <v>357</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>358</v>
+        <v>227</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>359</v>
+        <v>228</v>
       </c>
       <c r="E32" t="s" s="2">
-        <v>360</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>361</v>
+        <v>230</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>362</v>
+        <v>231</v>
       </c>
       <c r="E33" t="s" s="2">
-        <v>363</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>364</v>
+        <v>233</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>365</v>
+        <v>234</v>
       </c>
       <c r="E34" t="s" s="2">
-        <v>366</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>367</v>
+        <v>236</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>290</v>
+        <v>159</v>
       </c>
       <c r="E35" t="s" s="2">
-        <v>291</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>368</v>
+        <v>237</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D36" t="s" s="2">
-        <v>369</v>
+        <v>238</v>
       </c>
       <c r="E36" t="s" s="2">
-        <v>370</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>371</v>
+        <v>240</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>372</v>
+        <v>241</v>
       </c>
       <c r="E37" t="s" s="2">
-        <v>373</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>374</v>
+        <v>243</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D38" t="s" s="2">
-        <v>375</v>
+        <v>244</v>
       </c>
       <c r="E38" t="s" s="2">
-        <v>376</v>
+        <v>245</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>377</v>
+        <v>246</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>378</v>
+        <v>247</v>
       </c>
       <c r="E39" t="s" s="2">
-        <v>379</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>380</v>
+        <v>249</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D40" t="s" s="2">
-        <v>381</v>
+        <v>250</v>
       </c>
       <c r="E40" t="s" s="2">
-        <v>382</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>383</v>
+        <v>252</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>384</v>
+        <v>253</v>
       </c>
       <c r="E41" t="s" s="2">
-        <v>385</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>386</v>
+        <v>255</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D42" t="s" s="2">
-        <v>387</v>
+        <v>256</v>
       </c>
       <c r="E42" t="s" s="2">
-        <v>388</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>389</v>
+        <v>258</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>331</v>
+        <v>200</v>
       </c>
       <c r="E43" t="s" s="2">
-        <v>332</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>390</v>
+        <v>259</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D44" t="s" s="2">
-        <v>391</v>
+        <v>260</v>
       </c>
       <c r="E44" t="s" s="2">
-        <v>392</v>
+        <v>261</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>393</v>
+        <v>262</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D45" t="s" s="2">
-        <v>394</v>
+        <v>263</v>
       </c>
       <c r="E45" t="s" s="2">
-        <v>395</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>396</v>
+        <v>265</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D46" t="s" s="2">
-        <v>397</v>
+        <v>266</v>
       </c>
       <c r="E46" t="s" s="2">
-        <v>398</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>399</v>
+        <v>268</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D47" t="s" s="2">
-        <v>400</v>
+        <v>269</v>
       </c>
       <c r="E47" t="s" s="2">
-        <v>401</v>
+        <v>270</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>402</v>
+        <v>271</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D48" t="s" s="2">
-        <v>320</v>
+        <v>189</v>
       </c>
       <c r="E48" t="s" s="2">
-        <v>321</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>403</v>
+        <v>272</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>320</v>
+        <v>189</v>
       </c>
       <c r="E49" t="s" s="2">
-        <v>321</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>404</v>
+        <v>273</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>405</v>
+        <v>274</v>
       </c>
       <c r="E50" t="s" s="2">
-        <v>406</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>407</v>
+        <v>276</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D51" t="s" s="2">
-        <v>405</v>
+        <v>274</v>
       </c>
       <c r="E51" t="s" s="2">
-        <v>406</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>408</v>
+        <v>277</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D52" t="s" s="2">
-        <v>409</v>
+        <v>278</v>
       </c>
       <c r="E52" t="s" s="2">
-        <v>410</v>
+        <v>279</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>411</v>
+        <v>280</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D53" t="s" s="2">
-        <v>412</v>
+        <v>281</v>
       </c>
       <c r="E53" t="s" s="2">
-        <v>413</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>414</v>
+        <v>283</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
         <v>33</v>
       </c>
       <c r="D54" t="s" s="2">
-        <v>415</v>
+        <v>284</v>
       </c>
       <c r="E54" t="s" s="2">
-        <v>416</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>